<commit_message>
create logic to parse excel
</commit_message>
<xml_diff>
--- a/odk_remake/form_data/test/simple.xlsx
+++ b/odk_remake/form_data/test/simple.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Ariel\CSE482\odk_remake\form_data\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB43C5AF-DD00-4B88-85AE-A9DE62D16872}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1B4590-B8F7-408F-AD38-5D46B5498CC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3855" yWindow="3855" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38040" yWindow="3045" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -582,7 +582,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>type</t>
   </si>
@@ -639,9 +639,6 @@
   </si>
   <si>
     <t>video</t>
-  </si>
-  <si>
-    <t>integer</t>
   </si>
   <si>
     <t>age</t>
@@ -741,6 +738,12 @@
   </si>
   <si>
     <t>${graduate_year} = 2024</t>
+  </si>
+  <si>
+    <t>numeric</t>
+  </si>
+  <si>
+    <t>select_one abcd_icon</t>
   </si>
 </sst>
 </file>
@@ -1249,7 +1252,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1337,17 +1340,17 @@
     </row>
     <row r="2" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1375,17 +1378,17 @@
     </row>
     <row r="3" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>20</v>
-      </c>
       <c r="C3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
@@ -1413,20 +1416,20 @@
     </row>
     <row r="4" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>52</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -1453,20 +1456,20 @@
     </row>
     <row r="5" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
@@ -11048,7 +11051,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <conditionalFormatting sqref="A1:AB1 A14:AB1001 A4:AB12 A2:E3">
+  <conditionalFormatting sqref="A1:AB1 A2:E3 A4:AB12 A14:AB1001">
     <cfRule type="expression" dxfId="7" priority="1">
       <formula>OR($A1="begin group", $A1="begin_group", $A1="end group", $A1="end_group")</formula>
     </cfRule>
@@ -11056,20 +11059,20 @@
       <formula>OR($A1="begin repeat", $A1="begin_repeat", $A1="end repeat", $A1="end_repeat")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="F2:AB3">
+    <cfRule type="expression" dxfId="5" priority="9">
+      <formula>OR(#REF!="begin group", #REF!="begin_group", #REF!="end group", #REF!="end_group")</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="10">
+      <formula>OR(#REF!="begin repeat", #REF!="begin_repeat", #REF!="end repeat", #REF!="end_repeat")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="F13:AB13">
-    <cfRule type="expression" dxfId="5" priority="7">
+    <cfRule type="expression" dxfId="3" priority="7">
       <formula>OR($A2="begin group", $A2="begin_group", $A2="end group", $A2="end_group")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="8">
+    <cfRule type="expression" dxfId="2" priority="8">
       <formula>OR($A2="begin repeat", $A2="begin_repeat", $A2="end repeat", $A2="end_repeat")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F2:AB3">
-    <cfRule type="expression" dxfId="3" priority="9">
-      <formula>OR(#REF!="begin group", #REF!="begin_group", #REF!="end group", #REF!="end_group")</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="10">
-      <formula>OR(#REF!="begin repeat", #REF!="begin_repeat", #REF!="end repeat", #REF!="end_repeat")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -11111,7 +11114,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>1</v>
@@ -11147,16 +11150,16 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="6" t="s">
         <v>28</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>29</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -11183,16 +11186,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
@@ -11219,16 +11222,16 @@
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -11255,16 +11258,16 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -18132,22 +18135,22 @@
   <sheetData>
     <row r="1" spans="1:26" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>43</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>44</v>
       </c>
       <c r="G1" s="10"/>
       <c r="H1" s="10"/>
@@ -18175,7 +18178,7 @@
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="str">
         <f ca="1">TEXT(NOW(), "yyyymmddhhmmss")</f>
-        <v>20240422223217</v>
+        <v>20240427140610</v>
       </c>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>

</xml_diff>